<commit_message>
style: acomoda todo de nuevo
</commit_message>
<xml_diff>
--- a/docs/Correlacion.xlsx
+++ b/docs/Correlacion.xlsx
@@ -223,76 +223,76 @@
         <v>1.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.15178820180914482</v>
+        <v>0.15193166363410365</v>
       </c>
       <c r="D2" t="n">
-        <v>0.40235984115342166</v>
+        <v>0.4024163631242274</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.2613703895264798</v>
+        <v>-0.26136914956705654</v>
       </c>
       <c r="F2" t="n">
-        <v>0.08568134886886211</v>
+        <v>0.08567396187878927</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09406299277991532</v>
+        <v>0.0940530750326406</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8237211415329279</v>
+        <v>0.8238722432873298</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7459794421347599</v>
+        <v>0.7349644893289486</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9114327109620018</v>
+        <v>0.9115736614095262</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.2527398442423127</v>
+        <v>-0.25273429981618145</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08551689243117366</v>
+        <v>0.0855223849805489</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0751234618883194</v>
+        <v>0.07507187345534551</v>
       </c>
       <c r="N2" t="n">
-        <v>0.26586382609855896</v>
+        <v>0.2649912355622293</v>
       </c>
       <c r="O2" t="n">
-        <v>0.09897341363034219</v>
+        <v>0.09898073580391141</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7198610212217741</v>
+        <v>0.7199076399549454</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.41847481104010875</v>
+        <v>0.41841036656617514</v>
       </c>
       <c r="R2" t="n">
-        <v>0.668885338760564</v>
+        <v>0.6689584939287695</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7609142390384921</v>
+        <v>0.7608965599327245</v>
       </c>
       <c r="T2" t="n">
-        <v>0.663057849236512</v>
+        <v>0.6630712849446293</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8029844314142588</v>
+        <v>0.8029863325731461</v>
       </c>
       <c r="V2" t="n">
-        <v>0.2861588638797394</v>
+        <v>0.28617676272289555</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.08479198617028212</v>
+        <v>-0.08458782956211898</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.07302379821679111</v>
+        <v>-0.07284511030367655</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.08460270207281333</v>
+        <v>0.08455590777682177</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.4008635492248569</v>
+        <v>-0.4011099806689772</v>
       </c>
     </row>
     <row r="3">
@@ -300,79 +300,79 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.15178820180914482</v>
+        <v>0.15193166363410365</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.25287416241424043</v>
+        <v>0.25286605418939784</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03784493104691635</v>
+        <v>0.03786431356993579</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6187752636510666</v>
+        <v>0.6186671908127254</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5393209585439658</v>
+        <v>0.5392253551574553</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1982605937323838</v>
+        <v>0.19826409057912206</v>
       </c>
       <c r="I3" t="n">
-        <v>0.08902875659926299</v>
+        <v>0.08475633843868018</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1601325282375235</v>
+        <v>0.16015669423347648</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.24777560479207827</v>
+        <v>-0.24757342733345372</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.0139819714733911</v>
+        <v>-0.014011475909318123</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5539810099962037</v>
+        <v>0.5539502635758272</v>
       </c>
       <c r="N3" t="n">
-        <v>0.15895011606891815</v>
+        <v>0.15881967741018185</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.08062579327619145</v>
+        <v>-0.08067872575838148</v>
       </c>
       <c r="P3" t="n">
-        <v>0.2031807598329241</v>
+        <v>0.20296257443487184</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.2199599112020001</v>
+        <v>0.21955187010836053</v>
       </c>
       <c r="R3" t="n">
-        <v>0.19239018610836975</v>
+        <v>0.1922578398223046</v>
       </c>
       <c r="S3" t="n">
-        <v>0.21095931666232537</v>
+        <v>0.2103514687794412</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1309667387525537</v>
+        <v>0.1312054356926036</v>
       </c>
       <c r="U3" t="n">
-        <v>0.17682338925906219</v>
+        <v>0.17689659643524452</v>
       </c>
       <c r="V3" t="n">
-        <v>0.12397720396687362</v>
+        <v>0.12342536375189614</v>
       </c>
       <c r="W3" t="n">
-        <v>0.030130653466924312</v>
+        <v>0.030121489048508535</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.08372123645505845</v>
+        <v>-0.08353010852171934</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.1317082009992733</v>
+        <v>0.13194355810060088</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.1287168867134051</v>
+        <v>-0.12854336852620524</v>
       </c>
     </row>
     <row r="4">
@@ -380,79 +380,79 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.40235984115342166</v>
+        <v>0.4024163631242274</v>
       </c>
       <c r="C4" t="n">
-        <v>0.25287416241424043</v>
+        <v>0.25286605418939784</v>
       </c>
       <c r="D4" t="n">
         <v>1.0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1806827029738585</v>
+        <v>0.18072227230353563</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.034062875548522095</v>
+        <v>-0.034253816051520315</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07342890053074055</v>
+        <v>0.07320824707407643</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6570893948155517</v>
+        <v>0.657093862146251</v>
       </c>
       <c r="I4" t="n">
-        <v>0.20587040369582152</v>
+        <v>0.18767579623297218</v>
       </c>
       <c r="J4" t="n">
-        <v>0.47270212152273505</v>
+        <v>0.4726839840318307</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.5897679635994698</v>
+        <v>-0.5895197979131472</v>
       </c>
       <c r="L4" t="n">
-        <v>0.19923865292703524</v>
+        <v>0.1992782685888592</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.05460032427072144</v>
+        <v>-0.054627650722051606</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3915422837763535</v>
+        <v>0.3912074068938742</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.13325727258254347</v>
+        <v>-0.1332189519573308</v>
       </c>
       <c r="P4" t="n">
-        <v>0.6921545062746607</v>
+        <v>0.6919856593643237</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.8212436345063915</v>
+        <v>0.8209267117920817</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7409913728125943</v>
+        <v>0.7408899525340866</v>
       </c>
       <c r="S4" t="n">
-        <v>0.7409620516894665</v>
+        <v>0.7404885110111071</v>
       </c>
       <c r="T4" t="n">
-        <v>0.5303744040775561</v>
+        <v>0.5305627104623677</v>
       </c>
       <c r="U4" t="n">
-        <v>0.6175461410074543</v>
+        <v>0.6176050955657476</v>
       </c>
       <c r="V4" t="n">
-        <v>0.4286734730575572</v>
+        <v>0.4282428885074724</v>
       </c>
       <c r="W4" t="n">
-        <v>0.22525180084370286</v>
+        <v>0.22524543185423943</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.6216668100703879</v>
+        <v>-0.6215194847103886</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.3541034212667023</v>
+        <v>0.35428835451686685</v>
       </c>
       <c r="Z4" t="n">
-        <v>-0.4040967295033378</v>
+        <v>-0.403962001583791</v>
       </c>
     </row>
     <row r="5">
@@ -460,79 +460,79 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2613703895264798</v>
+        <v>-0.26136914956705654</v>
       </c>
       <c r="C5" t="n">
-        <v>0.03784493104691635</v>
+        <v>0.03786431356993579</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1806827029738585</v>
+        <v>0.18072227230353563</v>
       </c>
       <c r="E5" t="n">
         <v>1.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0327780775468991</v>
+        <v>0.03278172609462328</v>
       </c>
       <c r="G5" t="n">
-        <v>0.06033909695439854</v>
+        <v>0.06034470386514934</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.013132440524073117</v>
+        <v>-0.013194352158107369</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.07500272215025765</v>
+        <v>-0.07021553936951251</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.1742919145529678</v>
+        <v>-0.1744868333341813</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1171343471817348</v>
+        <v>-0.11713835008223378</v>
       </c>
       <c r="L5" t="n">
-        <v>0.08090236574063256</v>
+        <v>0.08090051761098734</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.013623116398655327</v>
+        <v>-0.013601636024778029</v>
       </c>
       <c r="N5" t="n">
-        <v>0.17037158421769297</v>
+        <v>0.17068435440825117</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.5241428156756738</v>
+        <v>-0.5241482125171177</v>
       </c>
       <c r="P5" t="n">
-        <v>0.044709836550658306</v>
+        <v>0.04469121278830977</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.17393718701820604</v>
+        <v>0.17396441728389117</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0991928950249189</v>
+        <v>0.09916322927525269</v>
       </c>
       <c r="S5" t="n">
-        <v>0.012673818616274783</v>
+        <v>0.012681909356761818</v>
       </c>
       <c r="T5" t="n">
-        <v>0.03471180636901893</v>
+        <v>0.0347068955340546</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.01738219990941913</v>
+        <v>-0.017382206999163766</v>
       </c>
       <c r="V5" t="n">
-        <v>0.31974103199419707</v>
+        <v>0.3197340145862147</v>
       </c>
       <c r="W5" t="n">
-        <v>0.21196029937779365</v>
+        <v>0.21187556600841595</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.09345381819554281</v>
+        <v>-0.09352809362705967</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.37100616318672514</v>
+        <v>0.3710258199189911</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.13793065523989362</v>
+        <v>-0.13782882248723416</v>
       </c>
     </row>
     <row r="6">
@@ -540,79 +540,79 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.08568134886886211</v>
+        <v>0.08567396187878927</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6187752636510666</v>
+        <v>0.6186671908127254</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.034062875548522095</v>
+        <v>-0.034253816051520315</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0327780775468991</v>
+        <v>0.03278172609462328</v>
       </c>
       <c r="F6" t="n">
         <v>1.0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.47739435685511505</v>
+        <v>0.47738453602684344</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0454961629056106</v>
+        <v>0.04575470388653489</v>
       </c>
       <c r="I6" t="n">
-        <v>0.06576770535828537</v>
+        <v>0.0696284899091743</v>
       </c>
       <c r="J6" t="n">
-        <v>0.056910222290631224</v>
+        <v>0.056843524935888824</v>
       </c>
       <c r="K6" t="n">
-        <v>0.014803255610963338</v>
+        <v>0.014816858874386139</v>
       </c>
       <c r="L6" t="n">
-        <v>9.135500867619533E-6</v>
+        <v>1.789392745322501E-5</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9747191733791062</v>
+        <v>0.9746364699624246</v>
       </c>
       <c r="N6" t="n">
-        <v>0.02853304168495199</v>
+        <v>0.028450170906007804</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.08188147165182905</v>
+        <v>-0.08187095677069421</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0017485067017838243</v>
+        <v>-0.0016707612131358106</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.020753365996418218</v>
+        <v>-0.02086679788706595</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.031142691689961102</v>
+        <v>-0.03101900471251593</v>
       </c>
       <c r="S6" t="n">
-        <v>0.00437375208185223</v>
+        <v>0.004340057281572</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.05523631691413752</v>
+        <v>-0.055216166178182945</v>
       </c>
       <c r="U6" t="n">
-        <v>0.04158958280799752</v>
+        <v>0.04158987793778277</v>
       </c>
       <c r="V6" t="n">
-        <v>0.11344960320315912</v>
+        <v>0.11348022264803917</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.03993830086440237</v>
+        <v>-0.03958479114431451</v>
       </c>
       <c r="X6" t="n">
-        <v>0.03003659867749984</v>
+        <v>0.0303464641101001</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.0262095765935437</v>
+        <v>0.026128403304239975</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.086782795635118</v>
+        <v>-0.08720840212673289</v>
       </c>
     </row>
     <row r="7">
@@ -620,79 +620,79 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.09406299277991532</v>
+        <v>0.0940530750326406</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5393209585439658</v>
+        <v>0.5392253551574553</v>
       </c>
       <c r="D7" t="n">
-        <v>0.07342890053074055</v>
+        <v>0.07320824707407643</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06033909695439854</v>
+        <v>0.06034470386514934</v>
       </c>
       <c r="F7" t="n">
-        <v>0.47739435685511505</v>
+        <v>0.47738453602684344</v>
       </c>
       <c r="G7" t="n">
         <v>1.0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.06664631414703481</v>
+        <v>0.0670075874710362</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1006864647507649</v>
+        <v>0.10193246633025822</v>
       </c>
       <c r="J7" t="n">
-        <v>0.08880013459744195</v>
+        <v>0.08870496606743415</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.20517343823482348</v>
+        <v>-0.20515886606481024</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.08852019947834908</v>
+        <v>-0.08850943948929031</v>
       </c>
       <c r="M7" t="n">
-        <v>0.43572194558673766</v>
+        <v>0.4356028991112492</v>
       </c>
       <c r="N7" t="n">
-        <v>0.13307753579321777</v>
+        <v>0.13303258518752728</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.04451527880605521</v>
+        <v>-0.04450008562798925</v>
       </c>
       <c r="P7" t="n">
-        <v>0.07255068960238202</v>
+        <v>0.07266020606940225</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.021094968429770673</v>
+        <v>0.02093716738284558</v>
       </c>
       <c r="R7" t="n">
-        <v>0.12744173749726836</v>
+        <v>0.12761641657697947</v>
       </c>
       <c r="S7" t="n">
-        <v>0.11235920242421685</v>
+        <v>0.11231368966347402</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1200672354350456</v>
+        <v>0.12009756281689278</v>
       </c>
       <c r="U7" t="n">
-        <v>0.05617918973131591</v>
+        <v>0.05617996612779553</v>
       </c>
       <c r="V7" t="n">
-        <v>0.057785053499223665</v>
+        <v>0.05782745907899716</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.021062041947654517</v>
+        <v>-0.020568602552664877</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.01743171977347412</v>
+        <v>-0.0169998302752807</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.07948336390242786</v>
+        <v>0.07937092269341771</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.11368666816695482</v>
+        <v>-0.11428132838583253</v>
       </c>
     </row>
     <row r="8">
@@ -700,46 +700,46 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8237211415329279</v>
+        <v>0.8238722432873298</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1982605937323838</v>
+        <v>0.19826409057912206</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6570893948155517</v>
+        <v>0.657093862146251</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.013132440524073117</v>
+        <v>-0.013194352158107369</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0454961629056106</v>
+        <v>0.04575470388653489</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06664631414703481</v>
+        <v>0.0670075874710362</v>
       </c>
       <c r="H8" t="n">
         <v>1.0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.6242633702929983</v>
+        <v>0.6110722975305887</v>
       </c>
       <c r="J8" t="n">
-        <v>0.836967357607809</v>
+        <v>0.8373103033386963</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.4319273539145221</v>
+        <v>-0.4321739688692924</v>
       </c>
       <c r="L8" t="n">
-        <v>0.17143304881428575</v>
+        <v>0.17127416345469104</v>
       </c>
       <c r="M8" t="n">
         <v>0.014076587996664494</v>
       </c>
       <c r="N8" t="n">
-        <v>0.37223735665543617</v>
+        <v>0.37186633106692785</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.020672573442085795</v>
+        <v>-0.02088145987633856</v>
       </c>
       <c r="P8" t="n">
         <v>0.8296204522561029</v>
@@ -780,79 +780,79 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7459794421347599</v>
+        <v>0.7349644893289486</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08902875659926299</v>
+        <v>0.08475633843868018</v>
       </c>
       <c r="D9" t="n">
-        <v>0.20587040369582152</v>
+        <v>0.18767579623297218</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.07500272215025765</v>
+        <v>-0.07021553936951251</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06576770535828537</v>
+        <v>0.0696284899091743</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1006864647507649</v>
+        <v>0.10193246633025822</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6242633702929983</v>
+        <v>0.6110722975305887</v>
       </c>
       <c r="I9" t="n">
         <v>1.0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6737489795500666</v>
+        <v>0.6633924528691536</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.1291457319186842</v>
+        <v>-0.11701146358484438</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0978437896454258</v>
+        <v>0.10046434382668716</v>
       </c>
       <c r="M9" t="n">
-        <v>0.034949587403975114</v>
+        <v>0.03945292759330184</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2420748834004012</v>
+        <v>0.22773554027698933</v>
       </c>
       <c r="O9" t="n">
-        <v>0.22453758562052328</v>
+        <v>0.2218534540498559</v>
       </c>
       <c r="P9" t="n">
-        <v>0.5620933661600227</v>
+        <v>0.5467331046847627</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.217728227090361</v>
+        <v>0.20085113283529385</v>
       </c>
       <c r="R9" t="n">
-        <v>0.4348375118587256</v>
+        <v>0.4206715471262043</v>
       </c>
       <c r="S9" t="n">
-        <v>0.557814202872538</v>
+        <v>0.5425080105807821</v>
       </c>
       <c r="T9" t="n">
-        <v>0.5505474689652798</v>
+        <v>0.5365834768646789</v>
       </c>
       <c r="U9" t="n">
-        <v>0.5921672646776562</v>
+        <v>0.5809706791059193</v>
       </c>
       <c r="V9" t="n">
-        <v>0.28948453663749796</v>
+        <v>0.28412005611371377</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.1706775204438243</v>
+        <v>-0.17330317079879684</v>
       </c>
       <c r="X9" t="n">
-        <v>0.01138195600611876</v>
+        <v>0.022711735795511532</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.15724953896708527</v>
+        <v>0.15882379646701883</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.38486318284748083</v>
+        <v>-0.3704353355022719</v>
       </c>
     </row>
     <row r="10">
@@ -860,79 +860,79 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9114327109620018</v>
+        <v>0.9115736614095262</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1601325282375235</v>
+        <v>0.16015669423347648</v>
       </c>
       <c r="D10" t="n">
-        <v>0.47270212152273505</v>
+        <v>0.4726839840318307</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1742919145529678</v>
+        <v>-0.1744868333341813</v>
       </c>
       <c r="F10" t="n">
-        <v>0.056910222290631224</v>
+        <v>0.056843524935888824</v>
       </c>
       <c r="G10" t="n">
-        <v>0.08880013459744195</v>
+        <v>0.08870496606743415</v>
       </c>
       <c r="H10" t="n">
-        <v>0.836967357607809</v>
+        <v>0.8373103033386963</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6737489795500666</v>
+        <v>0.6633924528691536</v>
       </c>
       <c r="J10" t="n">
         <v>1.0</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.29432912263829125</v>
+        <v>-0.29423315248022763</v>
       </c>
       <c r="L10" t="n">
-        <v>0.11581125784771791</v>
+        <v>0.11577431062799072</v>
       </c>
       <c r="M10" t="n">
-        <v>0.044454707390965104</v>
+        <v>0.04433122975022115</v>
       </c>
       <c r="N10" t="n">
-        <v>0.2976714813497182</v>
+        <v>0.2969498307461992</v>
       </c>
       <c r="O10" t="n">
-        <v>0.09063059518938278</v>
+        <v>0.0908379373418088</v>
       </c>
       <c r="P10" t="n">
-        <v>0.7868685993535798</v>
+        <v>0.7871960121598922</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.5226360704503551</v>
+        <v>0.522626064001739</v>
       </c>
       <c r="R10" t="n">
-        <v>0.7062895591238477</v>
+        <v>0.7063770716666301</v>
       </c>
       <c r="S10" t="n">
-        <v>0.8136831352977587</v>
+        <v>0.8138186876058502</v>
       </c>
       <c r="T10" t="n">
-        <v>0.6906067004997695</v>
+        <v>0.6906421227490411</v>
       </c>
       <c r="U10" t="n">
-        <v>0.8152201184667021</v>
+        <v>0.8153883006279398</v>
       </c>
       <c r="V10" t="n">
-        <v>0.33710008170718886</v>
+        <v>0.3369805379030569</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.0953149705146236</v>
+        <v>-0.09522344759233677</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.12790090418819364</v>
+        <v>-0.12749098654605362</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.15388177507481302</v>
+        <v>0.153620581343591</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.3691922648541773</v>
+        <v>-0.3694442735640953</v>
       </c>
     </row>
     <row r="11">
@@ -940,79 +940,79 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.2527398442423127</v>
+        <v>-0.25273429981618145</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.24777560479207827</v>
+        <v>-0.24757342733345372</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.5897679635994698</v>
+        <v>-0.5895197979131472</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.1171343471817348</v>
+        <v>-0.11713835008223378</v>
       </c>
       <c r="F11" t="n">
-        <v>0.014803255610963338</v>
+        <v>0.014816858874386139</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.20517343823482348</v>
+        <v>-0.20515886606481024</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.4319273539145221</v>
+        <v>-0.4321739688692924</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.1291457319186842</v>
+        <v>-0.11701146358484438</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.29432912263829125</v>
+        <v>-0.29423315248022763</v>
       </c>
       <c r="K11" t="n">
         <v>1.0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.03333950320005295</v>
+        <v>0.0333315323015619</v>
       </c>
       <c r="M11" t="n">
-        <v>0.02827258846651875</v>
+        <v>0.028357411615512088</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.3260964813841379</v>
+        <v>-0.32596388213514016</v>
       </c>
       <c r="O11" t="n">
-        <v>0.06212607020594785</v>
+        <v>0.0621159130653381</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.4354987366052451</v>
+        <v>-0.4355749338179919</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.5937331659733647</v>
+        <v>-0.5936299297640572</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.4967531896408344</v>
+        <v>-0.49687336223806877</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.43859750377546564</v>
+        <v>-0.4385684268984241</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.41094688554658454</v>
+        <v>-0.4109688889727198</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.41161743425799774</v>
+        <v>-0.4116200398367892</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.37846541939096806</v>
+        <v>-0.37849597407804314</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.2088144198274814</v>
+        <v>-0.20914989074688217</v>
       </c>
       <c r="X11" t="n">
-        <v>0.4945456912908103</v>
+        <v>0.4942563626777176</v>
       </c>
       <c r="Y11" t="n">
-        <v>-0.3244142009779126</v>
+        <v>-0.3243394126696966</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.29130401220609264</v>
+        <v>0.29170724964529177</v>
       </c>
     </row>
     <row r="12">
@@ -1020,79 +1020,79 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.08551689243117366</v>
+        <v>0.0855223849805489</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.0139819714733911</v>
+        <v>-0.014011475909318123</v>
       </c>
       <c r="D12" t="n">
-        <v>0.19923865292703524</v>
+        <v>0.1992782685888592</v>
       </c>
       <c r="E12" t="n">
-        <v>0.08090236574063256</v>
+        <v>0.08090051761098734</v>
       </c>
       <c r="F12" t="n">
-        <v>9.135500867619533E-6</v>
+        <v>1.789392745322501E-5</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.08852019947834908</v>
+        <v>-0.08850943948929031</v>
       </c>
       <c r="H12" t="n">
-        <v>0.17143304881428575</v>
+        <v>0.17127416345469104</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0978437896454258</v>
+        <v>0.10046434382668716</v>
       </c>
       <c r="J12" t="n">
-        <v>0.11581125784771791</v>
+        <v>0.11577431062799072</v>
       </c>
       <c r="K12" t="n">
-        <v>0.03333950320005295</v>
+        <v>0.0333315323015619</v>
       </c>
       <c r="L12" t="n">
         <v>1.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0052816412666317845</v>
+        <v>0.005336960978849341</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.12144019907718483</v>
+        <v>-0.12151970782931802</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.11359891709598549</v>
+        <v>-0.11360683297208773</v>
       </c>
       <c r="P12" t="n">
-        <v>0.12661306609578202</v>
+        <v>0.12656542318608524</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.16635682569770288</v>
+        <v>0.1664271841834162</v>
       </c>
       <c r="R12" t="n">
-        <v>0.0853107254045437</v>
+        <v>0.08523449126640081</v>
       </c>
       <c r="S12" t="n">
-        <v>0.17448381406021057</v>
+        <v>0.1745050980949839</v>
       </c>
       <c r="T12" t="n">
-        <v>0.06762778241862603</v>
+        <v>0.06761528809530261</v>
       </c>
       <c r="U12" t="n">
-        <v>0.1765163019025454</v>
+        <v>0.1765167789235841</v>
       </c>
       <c r="V12" t="n">
-        <v>0.15065951596736848</v>
+        <v>0.1506415244011129</v>
       </c>
       <c r="W12" t="n">
-        <v>0.1054230402401797</v>
+        <v>0.10520499633194716</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.29939883880357515</v>
+        <v>-0.29959073701167027</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.05280640691096568</v>
+        <v>0.052856757131522276</v>
       </c>
       <c r="Z12" t="n">
-        <v>-0.14986151306724793</v>
+        <v>-0.14959965263942152</v>
       </c>
     </row>
     <row r="13">
@@ -1100,46 +1100,46 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0751234618883194</v>
+        <v>0.07507187345534551</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5539810099962037</v>
+        <v>0.5539502635758272</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.05460032427072144</v>
+        <v>-0.054627650722051606</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.013623116398655327</v>
+        <v>-0.013601636024778029</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9747191733791062</v>
+        <v>0.9746364699624246</v>
       </c>
       <c r="G13" t="n">
-        <v>0.43572194558673766</v>
+        <v>0.4356028991112492</v>
       </c>
       <c r="H13" t="n">
         <v>0.014076587996664494</v>
       </c>
       <c r="I13" t="n">
-        <v>0.034949587403975114</v>
+        <v>0.03945292759330184</v>
       </c>
       <c r="J13" t="n">
-        <v>0.044454707390965104</v>
+        <v>0.04433122975022115</v>
       </c>
       <c r="K13" t="n">
-        <v>0.02827258846651875</v>
+        <v>0.028357411615512088</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0052816412666317845</v>
+        <v>0.005336960978849341</v>
       </c>
       <c r="M13" t="n">
         <v>1.0</v>
       </c>
       <c r="N13" t="n">
-        <v>9.7429601054236E-4</v>
+        <v>8.16606447336251E-4</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.07013515247935949</v>
+        <v>-0.07006301254917342</v>
       </c>
       <c r="P13" t="n">
         <v>-0.0341622270864396</v>
@@ -1180,79 +1180,79 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.26586382609855896</v>
+        <v>0.2649912355622293</v>
       </c>
       <c r="C14" t="n">
-        <v>0.15895011606891815</v>
+        <v>0.15881967741018185</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3915422837763535</v>
+        <v>0.3912074068938742</v>
       </c>
       <c r="E14" t="n">
-        <v>0.17037158421769297</v>
+        <v>0.17068435440825117</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02853304168495199</v>
+        <v>0.028450170906007804</v>
       </c>
       <c r="G14" t="n">
-        <v>0.13307753579321777</v>
+        <v>0.13303258518752728</v>
       </c>
       <c r="H14" t="n">
-        <v>0.37223735665543617</v>
+        <v>0.37186633106692785</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2420748834004012</v>
+        <v>0.22773554027698933</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2976714813497182</v>
+        <v>0.2969498307461992</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.3260964813841379</v>
+        <v>-0.32596388213514016</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.12144019907718483</v>
+        <v>-0.12151970782931802</v>
       </c>
       <c r="M14" t="n">
-        <v>9.7429601054236E-4</v>
+        <v>8.16606447336251E-4</v>
       </c>
       <c r="N14" t="n">
         <v>1.0</v>
       </c>
       <c r="O14" t="n">
-        <v>0.017474621147214018</v>
+        <v>0.017761068677049793</v>
       </c>
       <c r="P14" t="n">
-        <v>0.5239784542532273</v>
+        <v>0.5235550406041395</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.5082124535165571</v>
+        <v>0.5076338188225815</v>
       </c>
       <c r="R14" t="n">
-        <v>0.4183422856808661</v>
+        <v>0.4178839925276908</v>
       </c>
       <c r="S14" t="n">
-        <v>0.46812261791163706</v>
+        <v>0.4680960322291072</v>
       </c>
       <c r="T14" t="n">
-        <v>0.4613180674205351</v>
+        <v>0.46075230487427</v>
       </c>
       <c r="U14" t="n">
-        <v>0.38593547187356164</v>
+        <v>0.38547552005999597</v>
       </c>
       <c r="V14" t="n">
-        <v>0.19825615345223147</v>
+        <v>0.19753563386839837</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.1510720968571224</v>
+        <v>-0.15072958826214836</v>
       </c>
       <c r="X14" t="n">
-        <v>-0.09866943994796974</v>
+        <v>-0.09833910460958849</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.1114056294927507</v>
+        <v>0.11105607610764806</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.37858106422176047</v>
+        <v>-0.37823939841170795</v>
       </c>
     </row>
     <row r="15">
@@ -1260,79 +1260,79 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.09897341363034219</v>
+        <v>0.09898073580391141</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.08062579327619145</v>
+        <v>-0.08067872575838148</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.13325727258254347</v>
+        <v>-0.1332189519573308</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.5241428156756738</v>
+        <v>-0.5241482125171177</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.08188147165182905</v>
+        <v>-0.08187095677069421</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.04451527880605521</v>
+        <v>-0.04450008562798925</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.020672573442085795</v>
+        <v>-0.02088145987633856</v>
       </c>
       <c r="I15" t="n">
-        <v>0.22453758562052328</v>
+        <v>0.2218534540498559</v>
       </c>
       <c r="J15" t="n">
-        <v>0.09063059518938278</v>
+        <v>0.0908379373418088</v>
       </c>
       <c r="K15" t="n">
-        <v>0.06212607020594785</v>
+        <v>0.0621159130653381</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.11359891709598549</v>
+        <v>-0.11360683297208773</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.07013515247935949</v>
+        <v>-0.07006301254917342</v>
       </c>
       <c r="N15" t="n">
-        <v>0.017474621147214018</v>
+        <v>0.017761068677049793</v>
       </c>
       <c r="O15" t="n">
         <v>1.0</v>
       </c>
       <c r="P15" t="n">
-        <v>0.046733000279357485</v>
+        <v>0.04667034346725342</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.04753440127862168</v>
+        <v>-0.04744302191693503</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.19477545296960982</v>
+        <v>-0.19487654639555677</v>
       </c>
       <c r="S15" t="n">
-        <v>0.06129383731875354</v>
+        <v>0.06132139179938568</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.053933561417596095</v>
+        <v>-0.053950422107609544</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.062342319600954044</v>
+        <v>-0.062342608842098114</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.3204279308536053</v>
+        <v>-0.3204535248684406</v>
       </c>
       <c r="W15" t="n">
-        <v>-0.3548057114006418</v>
+        <v>-0.3550934282905189</v>
       </c>
       <c r="X15" t="n">
-        <v>0.09026284619178242</v>
+        <v>0.09001288571804851</v>
       </c>
       <c r="Y15" t="n">
-        <v>-0.30403301692223256</v>
+        <v>-0.3039686418570449</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.10908617659839087</v>
+        <v>0.10943032249395479</v>
       </c>
     </row>
     <row r="16">
@@ -1340,46 +1340,46 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.7198610212217741</v>
+        <v>0.7199076399549454</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2031807598329241</v>
+        <v>0.20296257443487184</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6921545062746607</v>
+        <v>0.6919856593643237</v>
       </c>
       <c r="E16" t="n">
-        <v>0.044709836550658306</v>
+        <v>0.04469121278830977</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0017485067017838243</v>
+        <v>-0.0016707612131358106</v>
       </c>
       <c r="G16" t="n">
-        <v>0.07255068960238202</v>
+        <v>0.07266020606940225</v>
       </c>
       <c r="H16" t="n">
         <v>0.8296204522561029</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5620933661600227</v>
+        <v>0.5467331046847627</v>
       </c>
       <c r="J16" t="n">
-        <v>0.7868685993535798</v>
+        <v>0.7871960121598922</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.4354987366052451</v>
+        <v>-0.4355749338179919</v>
       </c>
       <c r="L16" t="n">
-        <v>0.12661306609578202</v>
+        <v>0.12656542318608524</v>
       </c>
       <c r="M16" t="n">
         <v>-0.0341622270864396</v>
       </c>
       <c r="N16" t="n">
-        <v>0.5239784542532273</v>
+        <v>0.5235550406041395</v>
       </c>
       <c r="O16" t="n">
-        <v>0.046733000279357485</v>
+        <v>0.04667034346725342</v>
       </c>
       <c r="P16" t="n">
         <v>1.0</v>
@@ -1420,46 +1420,46 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.41847481104010875</v>
+        <v>0.41841036656617514</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2199599112020001</v>
+        <v>0.21955187010836053</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8212436345063915</v>
+        <v>0.8209267117920817</v>
       </c>
       <c r="E17" t="n">
-        <v>0.17393718701820604</v>
+        <v>0.17396441728389117</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.020753365996418218</v>
+        <v>-0.02086679788706595</v>
       </c>
       <c r="G17" t="n">
-        <v>0.021094968429770673</v>
+        <v>0.02093716738284558</v>
       </c>
       <c r="H17" t="n">
         <v>0.6692070327662389</v>
       </c>
       <c r="I17" t="n">
-        <v>0.217728227090361</v>
+        <v>0.20085113283529385</v>
       </c>
       <c r="J17" t="n">
-        <v>0.5226360704503551</v>
+        <v>0.522626064001739</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.5937331659733647</v>
+        <v>-0.5936299297640572</v>
       </c>
       <c r="L17" t="n">
-        <v>0.16635682569770288</v>
+        <v>0.1664271841834162</v>
       </c>
       <c r="M17" t="n">
         <v>-0.03884806373697036</v>
       </c>
       <c r="N17" t="n">
-        <v>0.5082124535165571</v>
+        <v>0.5076338188225815</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.04753440127862168</v>
+        <v>-0.04744302191693503</v>
       </c>
       <c r="P17" t="n">
         <v>0.7326700818706109</v>
@@ -1500,46 +1500,46 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.668885338760564</v>
+        <v>0.6689584939287695</v>
       </c>
       <c r="C18" t="n">
-        <v>0.19239018610836975</v>
+        <v>0.1922578398223046</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7409913728125943</v>
+        <v>0.7408899525340866</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0991928950249189</v>
+        <v>0.09916322927525269</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.031142691689961102</v>
+        <v>-0.03101900471251593</v>
       </c>
       <c r="G18" t="n">
-        <v>0.12744173749726836</v>
+        <v>0.12761641657697947</v>
       </c>
       <c r="H18" t="n">
         <v>0.7891533711517214</v>
       </c>
       <c r="I18" t="n">
-        <v>0.4348375118587256</v>
+        <v>0.4206715471262043</v>
       </c>
       <c r="J18" t="n">
-        <v>0.7062895591238477</v>
+        <v>0.7063770716666301</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.4967531896408344</v>
+        <v>-0.49687336223806877</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0853107254045437</v>
+        <v>0.08523449126640081</v>
       </c>
       <c r="M18" t="n">
         <v>-0.06196215844947839</v>
       </c>
       <c r="N18" t="n">
-        <v>0.4183422856808661</v>
+        <v>0.4178839925276908</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.19477545296960982</v>
+        <v>-0.19487654639555677</v>
       </c>
       <c r="P18" t="n">
         <v>0.8163636092768212</v>
@@ -1580,46 +1580,46 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.7609142390384921</v>
+        <v>0.7608965599327245</v>
       </c>
       <c r="C19" t="n">
-        <v>0.21095931666232537</v>
+        <v>0.2103514687794412</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7409620516894665</v>
+        <v>0.7404885110111071</v>
       </c>
       <c r="E19" t="n">
-        <v>0.012673818616274783</v>
+        <v>0.012681909356761818</v>
       </c>
       <c r="F19" t="n">
-        <v>0.00437375208185223</v>
+        <v>0.004340057281572</v>
       </c>
       <c r="G19" t="n">
-        <v>0.11235920242421685</v>
+        <v>0.11231368966347402</v>
       </c>
       <c r="H19" t="n">
         <v>0.8600057019398789</v>
       </c>
       <c r="I19" t="n">
-        <v>0.557814202872538</v>
+        <v>0.5425080105807821</v>
       </c>
       <c r="J19" t="n">
-        <v>0.8136831352977587</v>
+        <v>0.8138186876058502</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.43859750377546564</v>
+        <v>-0.4385684268984241</v>
       </c>
       <c r="L19" t="n">
-        <v>0.17448381406021057</v>
+        <v>0.1745050980949839</v>
       </c>
       <c r="M19" t="n">
         <v>-0.022261997797862573</v>
       </c>
       <c r="N19" t="n">
-        <v>0.46812261791163706</v>
+        <v>0.4680960322291072</v>
       </c>
       <c r="O19" t="n">
-        <v>0.06129383731875354</v>
+        <v>0.06132139179938568</v>
       </c>
       <c r="P19" t="n">
         <v>0.9219399027824564</v>
@@ -1660,46 +1660,46 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.663057849236512</v>
+        <v>0.6630712849446293</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1309667387525537</v>
+        <v>0.1312054356926036</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5303744040775561</v>
+        <v>0.5305627104623677</v>
       </c>
       <c r="E20" t="n">
-        <v>0.03471180636901893</v>
+        <v>0.0347068955340546</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.05523631691413752</v>
+        <v>-0.055216166178182945</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1200672354350456</v>
+        <v>0.12009756281689278</v>
       </c>
       <c r="H20" t="n">
         <v>0.6925847829486167</v>
       </c>
       <c r="I20" t="n">
-        <v>0.5505474689652798</v>
+        <v>0.5365834768646789</v>
       </c>
       <c r="J20" t="n">
-        <v>0.6906067004997695</v>
+        <v>0.6906421227490411</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.41094688554658454</v>
+        <v>-0.4109688889727198</v>
       </c>
       <c r="L20" t="n">
-        <v>0.06762778241862603</v>
+        <v>0.06761528809530261</v>
       </c>
       <c r="M20" t="n">
         <v>-0.0928608437095917</v>
       </c>
       <c r="N20" t="n">
-        <v>0.4613180674205351</v>
+        <v>0.46075230487427</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.053933561417596095</v>
+        <v>-0.053950422107609544</v>
       </c>
       <c r="P20" t="n">
         <v>0.7328636168398585</v>
@@ -1740,46 +1740,46 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.8029844314142588</v>
+        <v>0.8029863325731461</v>
       </c>
       <c r="C21" t="n">
-        <v>0.17682338925906219</v>
+        <v>0.17689659643524452</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6175461410074543</v>
+        <v>0.6176050955657476</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.01738219990941913</v>
+        <v>-0.017382206999163766</v>
       </c>
       <c r="F21" t="n">
-        <v>0.04158958280799752</v>
+        <v>0.04158987793778277</v>
       </c>
       <c r="G21" t="n">
-        <v>0.05617918973131591</v>
+        <v>0.05617996612779553</v>
       </c>
       <c r="H21" t="n">
         <v>0.9675746001702192</v>
       </c>
       <c r="I21" t="n">
-        <v>0.5921672646776562</v>
+        <v>0.5809706791059193</v>
       </c>
       <c r="J21" t="n">
-        <v>0.8152201184667021</v>
+        <v>0.8153883006279398</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.41161743425799774</v>
+        <v>-0.4116200398367892</v>
       </c>
       <c r="L21" t="n">
-        <v>0.1765163019025454</v>
+        <v>0.1765167789235841</v>
       </c>
       <c r="M21" t="n">
         <v>0.0074615245624678845</v>
       </c>
       <c r="N21" t="n">
-        <v>0.38593547187356164</v>
+        <v>0.38547552005999597</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.062342319600954044</v>
+        <v>-0.062342608842098114</v>
       </c>
       <c r="P21" t="n">
         <v>0.7976595088675659</v>
@@ -1820,46 +1820,46 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.2861588638797394</v>
+        <v>0.28617676272289555</v>
       </c>
       <c r="C22" t="n">
-        <v>0.12397720396687362</v>
+        <v>0.12342536375189614</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4286734730575572</v>
+        <v>0.4282428885074724</v>
       </c>
       <c r="E22" t="n">
-        <v>0.31974103199419707</v>
+        <v>0.3197340145862147</v>
       </c>
       <c r="F22" t="n">
-        <v>0.11344960320315912</v>
+        <v>0.11348022264803917</v>
       </c>
       <c r="G22" t="n">
-        <v>0.057785053499223665</v>
+        <v>0.05782745907899716</v>
       </c>
       <c r="H22" t="n">
         <v>0.3892021557968771</v>
       </c>
       <c r="I22" t="n">
-        <v>0.28948453663749796</v>
+        <v>0.28412005611371377</v>
       </c>
       <c r="J22" t="n">
-        <v>0.33710008170718886</v>
+        <v>0.3369805379030569</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.37846541939096806</v>
+        <v>-0.37849597407804314</v>
       </c>
       <c r="L22" t="n">
-        <v>0.15065951596736848</v>
+        <v>0.1506415244011129</v>
       </c>
       <c r="M22" t="n">
         <v>0.09747728448388304</v>
       </c>
       <c r="N22" t="n">
-        <v>0.19825615345223147</v>
+        <v>0.19753563386839837</v>
       </c>
       <c r="O22" t="n">
-        <v>-0.3204279308536053</v>
+        <v>-0.3204535248684406</v>
       </c>
       <c r="P22" t="n">
         <v>0.4096539265219658</v>
@@ -1900,46 +1900,46 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.08479198617028212</v>
+        <v>-0.08458782956211898</v>
       </c>
       <c r="C23" t="n">
-        <v>0.030130653466924312</v>
+        <v>0.030121489048508535</v>
       </c>
       <c r="D23" t="n">
-        <v>0.22525180084370286</v>
+        <v>0.22524543185423943</v>
       </c>
       <c r="E23" t="n">
-        <v>0.21196029937779365</v>
+        <v>0.21187556600841595</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.03993830086440237</v>
+        <v>-0.03958479114431451</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.021062041947654517</v>
+        <v>-0.020568602552664877</v>
       </c>
       <c r="H23" t="n">
         <v>0.014091803911765958</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.1706775204438243</v>
+        <v>-0.17330317079879684</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.0953149705146236</v>
+        <v>-0.09522344759233677</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.2088144198274814</v>
+        <v>-0.20914989074688217</v>
       </c>
       <c r="L23" t="n">
-        <v>0.1054230402401797</v>
+        <v>0.10520499633194716</v>
       </c>
       <c r="M23" t="n">
         <v>-0.029348436638799567</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.1510720968571224</v>
+        <v>-0.15072958826214836</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.3548057114006418</v>
+        <v>-0.3550934282905189</v>
       </c>
       <c r="P23" t="n">
         <v>-0.06255645424593269</v>
@@ -1980,46 +1980,46 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.07302379821679111</v>
+        <v>-0.07284511030367655</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.08372123645505845</v>
+        <v>-0.08353010852171934</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.6216668100703879</v>
+        <v>-0.6215194847103886</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.09345381819554281</v>
+        <v>-0.09352809362705967</v>
       </c>
       <c r="F24" t="n">
-        <v>0.03003659867749984</v>
+        <v>0.0303464641101001</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.01743171977347412</v>
+        <v>-0.0169998302752807</v>
       </c>
       <c r="H24" t="n">
         <v>-0.2801629473829435</v>
       </c>
       <c r="I24" t="n">
-        <v>0.01138195600611876</v>
+        <v>0.022711735795511532</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.12790090418819364</v>
+        <v>-0.12749098654605362</v>
       </c>
       <c r="K24" t="n">
-        <v>0.4945456912908103</v>
+        <v>0.4942563626777176</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.29939883880357515</v>
+        <v>-0.29959073701167027</v>
       </c>
       <c r="M24" t="n">
         <v>0.03727040232849405</v>
       </c>
       <c r="N24" t="n">
-        <v>-0.09866943994796974</v>
+        <v>-0.09833910460958849</v>
       </c>
       <c r="O24" t="n">
-        <v>0.09026284619178242</v>
+        <v>0.09001288571804851</v>
       </c>
       <c r="P24" t="n">
         <v>-0.23201804806442144</v>
@@ -2060,46 +2060,46 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.08460270207281333</v>
+        <v>0.08455590777682177</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1317082009992733</v>
+        <v>0.13194355810060088</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3541034212667023</v>
+        <v>0.35428835451686685</v>
       </c>
       <c r="E25" t="n">
-        <v>0.37100616318672514</v>
+        <v>0.3710258199189911</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0262095765935437</v>
+        <v>0.026128403304239975</v>
       </c>
       <c r="G25" t="n">
-        <v>0.07948336390242786</v>
+        <v>0.07937092269341771</v>
       </c>
       <c r="H25" t="n">
         <v>0.2032319367615462</v>
       </c>
       <c r="I25" t="n">
-        <v>0.15724953896708527</v>
+        <v>0.15882379646701883</v>
       </c>
       <c r="J25" t="n">
-        <v>0.15388177507481302</v>
+        <v>0.153620581343591</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.3244142009779126</v>
+        <v>-0.3243394126696966</v>
       </c>
       <c r="L25" t="n">
-        <v>0.05280640691096568</v>
+        <v>0.052856757131522276</v>
       </c>
       <c r="M25" t="n">
         <v>-4.5622569097599993E-4</v>
       </c>
       <c r="N25" t="n">
-        <v>0.1114056294927507</v>
+        <v>0.11105607610764806</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.30403301692223256</v>
+        <v>-0.3039686418570449</v>
       </c>
       <c r="P25" t="n">
         <v>0.3060140067542387</v>
@@ -2140,46 +2140,46 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.4008635492248569</v>
+        <v>-0.4011099806689772</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.1287168867134051</v>
+        <v>-0.12854336852620524</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.4040967295033378</v>
+        <v>-0.403962001583791</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.13793065523989362</v>
+        <v>-0.13782882248723416</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.086782795635118</v>
+        <v>-0.08720840212673289</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.11368666816695482</v>
+        <v>-0.11428132838583253</v>
       </c>
       <c r="H26" t="n">
         <v>-0.4341566041716615</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.38486318284748083</v>
+        <v>-0.3704353355022719</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.3691922648541773</v>
+        <v>-0.3694442735640953</v>
       </c>
       <c r="K26" t="n">
-        <v>0.29130401220609264</v>
+        <v>0.29170724964529177</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.14986151306724793</v>
+        <v>-0.14959965263942152</v>
       </c>
       <c r="M26" t="n">
         <v>-0.048271099327374126</v>
       </c>
       <c r="N26" t="n">
-        <v>-0.37858106422176047</v>
+        <v>-0.37823939841170795</v>
       </c>
       <c r="O26" t="n">
-        <v>0.10908617659839087</v>
+        <v>0.10943032249395479</v>
       </c>
       <c r="P26" t="n">
         <v>-0.4820619657939511</v>

</xml_diff>